<commit_message>
updates frequencies.xlsx, changed false pos and neg counts to rates, cleaned up code, 99.9% done with the project
</commit_message>
<xml_diff>
--- a/project4/frequencies.xlsx
+++ b/project4/frequencies.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="THE_DATA" localSheetId="0">Sheet1!$A$1:$HU$6</definedName>
@@ -28,7 +28,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="THE_DATA" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" name="THE_DATA1" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="1257" sourceFile="C:\Users\kingsman142\Desktop\CS1571\project4\THE_DATA.txt" tab="0" delimiter="|">
       <textFields count="229">
         <textField/>
@@ -995,8 +995,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1311,9 +1339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HU6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2433,16 +2459,16 @@
         <v>5.91928251121E-2</v>
       </c>
       <c r="BN2">
-        <v>0.65241379310299996</v>
+        <v>0.65586206896599997</v>
       </c>
       <c r="BO2">
-        <v>0.34758620689699998</v>
+        <v>0.34413793103399998</v>
       </c>
       <c r="BP2">
-        <v>0.92242152466399996</v>
+        <v>0.92421524663700005</v>
       </c>
       <c r="BQ2">
-        <v>7.7578475336299996E-2</v>
+        <v>7.5784753363199994E-2</v>
       </c>
       <c r="BR2">
         <v>0.67241379310299998</v>
@@ -3122,16 +3148,16 @@
         <v>5.7821604661600003E-2</v>
       </c>
       <c r="BN3">
-        <v>0.64620689655200003</v>
+        <v>0.64896551724100004</v>
       </c>
       <c r="BO3">
-        <v>0.35379310344800002</v>
+        <v>0.35103448275900001</v>
       </c>
       <c r="BP3">
-        <v>0.92469744509200003</v>
+        <v>0.92649036306599997</v>
       </c>
       <c r="BQ3">
-        <v>7.5302554908100006E-2</v>
+        <v>7.3509636934099995E-2</v>
       </c>
       <c r="BR3">
         <v>0.66758620689699999</v>
@@ -3811,16 +3837,16 @@
         <v>6.0959211116099997E-2</v>
       </c>
       <c r="BN4">
-        <v>0.65172413793100004</v>
+        <v>0.656551724138</v>
       </c>
       <c r="BO4">
-        <v>0.34827586206900002</v>
+        <v>0.343448275862</v>
       </c>
       <c r="BP4">
-        <v>0.92380098610500005</v>
+        <v>0.92604213357200005</v>
       </c>
       <c r="BQ4">
-        <v>7.6199013895100004E-2</v>
+        <v>7.3957866427599994E-2</v>
       </c>
       <c r="BR4">
         <v>0.67931034482800001</v>
@@ -4500,16 +4526,16 @@
         <v>6.1883408071700001E-2</v>
       </c>
       <c r="BN5">
-        <v>0.66436940041400006</v>
+        <v>0.66850447966899995</v>
       </c>
       <c r="BO5">
-        <v>0.335630599586</v>
+        <v>0.33149552033099999</v>
       </c>
       <c r="BP5">
-        <v>0.92421524663700005</v>
+        <v>0.92645739910299996</v>
       </c>
       <c r="BQ5">
-        <v>7.5784753363199994E-2</v>
+        <v>7.3542600896899998E-2</v>
       </c>
       <c r="BR5">
         <v>0.68573397656799995</v>
@@ -5189,16 +5215,16 @@
         <v>5.7847533632299997E-2</v>
       </c>
       <c r="BN6">
-        <v>0.66988283942100002</v>
+        <v>0.67401791867700001</v>
       </c>
       <c r="BO6">
-        <v>0.33011716057899998</v>
+        <v>0.32598208132299999</v>
       </c>
       <c r="BP6">
-        <v>0.92825112107600005</v>
+        <v>0.92914798206299998</v>
       </c>
       <c r="BQ6">
-        <v>7.1748878923799997E-2</v>
+        <v>7.0852017937200001E-2</v>
       </c>
       <c r="BR6">
         <v>0.676085458305</v>

</xml_diff>